<commit_message>
propuesta, presentación y general full
</commit_message>
<xml_diff>
--- a/propuesta fundemerca.xlsx
+++ b/propuesta fundemerca.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cantidad inicial" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="85">
   <si>
     <t>Cód</t>
   </si>
@@ -276,6 +276,15 @@
   <si>
     <t>PROBABILIDAD</t>
   </si>
+  <si>
+    <t>Marca de clase</t>
+  </si>
+  <si>
+    <t>flexible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exigente </t>
+  </si>
 </sst>
 </file>
 
@@ -365,26 +374,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFCC99"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -459,7 +473,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5430,7 +5443,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5537,7 +5549,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10508,7 +10519,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16380,6 +16390,1640 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>INTERVALOS FLEXIBLES</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intervalos propuestos'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inferior</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intervalos propuestos'!$C$3:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>9.7788152551082606E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0581631174453454E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1754046717507276E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2428363815292233E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0020640545174228E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0000451058836728E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0466577968975184E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2810853173733503E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8405081358488655E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.180265033409368E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3798118951068071E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.503385333038859E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6969719322400365E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0521720534539213E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2065222154757494E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2830696306044517E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.1343993354656428E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.3460181046352338E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.3265827355353501E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3782054174299683E-5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.4870021380749694E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.9824077603693131E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.9580120086738468E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6867875816285214E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.8293768220318581E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.4220173564151612E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.0955613625522732E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.4035753845365116E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.4979976844291159E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.1155165317512842E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0466787871979192E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.0867700627293417E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0595299369769424E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.573168907624995E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4699745082761991E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.3236475204520384E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.1334534236819788E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.134472959163948E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0085502919607348E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.9580120086738468E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.5331462364387463E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.7600948455265265E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9.1343993354656428E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.0020640545174228E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.8840192997293E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9.1304019438005219E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.1112430356061909E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.2389613390461286E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-16A8-4896-8F25-53EA7AADCB98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intervalos propuestos'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Superior</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intervalos propuestos'!$D$3:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>8.5913877215295975E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9117242344121874E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7318606749461773E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10037325114945084</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7545953319678831E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11155978396773025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.1052604365895777E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3201112315604324E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14119004715724803</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.3753696224667773E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5245988168233229E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15441677682749588</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11789028780157729</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.7327671070721693E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.996780784975043E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.0369036165242602E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.4432235631596733E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.10313654794550842</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.7705555294467747E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.054415466789421E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.357589266390129E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.12247071822539768</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.6702967402606625E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.4783418224861333E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.6321410568283343E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10067736645664904</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.1460393991038336E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.9076258183104939E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.3365474637230421E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.4062077258677426E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.2837734257360953E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.4569622773026247E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.11864461620810685</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.8032760806448258E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.2622259618890914E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.3021956893641549E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.9639356455248547E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.2293243542040022E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.12840007592700819</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.11411080486394343</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.5872048118610156E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.9836260610489114E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.10917044329418557</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.4778570673349143E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.6899429082496567E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.8642413598954963E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.6668813796111004E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.10214242378704463</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-16A8-4896-8F25-53EA7AADCB98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intervalos propuestos'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>flexible</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intervalos propuestos'!$G$3:$G$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>4.784634623520212E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4849436759287667E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9536326733484527E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6400807482371536E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8783296932426527E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0780117513283494E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.075959116743548E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3741098816488839E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5015277646548445E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.2778173279380725E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4522053559650649E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.9960081080267364E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.7430003561988833E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.3924695802630455E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.1016515002253964E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.6599866235643557E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1783317483531188E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.6241283025071823E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.9516069015001548E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.5278968361034252E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6531447400988126E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.62265629928835E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.233048970564024E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.0825647020573272E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9575393695157599E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.744877001040033E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.9277977676795301E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.1556006014235031E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.7431736160829766E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.5588796895214355E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.1652261064670071E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3828196417877793E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.4619957788938129E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.2302964857036626E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.3046117063583557E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.3129216049080966E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.048694534603417E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.6818986566839754E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.9242789423307777E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.103440843630864E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.0601755241498812E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.8718604532877187E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.9152421314825607E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.2399605609261683E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.9391724191112932E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.3886407771377742E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.8890622076086456E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.7266018588752958E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-16A8-4896-8F25-53EA7AADCB98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:axId val="441982416"/>
+        <c:axId val="441981168"/>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="441982416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441981168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="441981168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441982416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>INTERVALOS EXIGENTES</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:stockChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intervalos propuestos'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inferior</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intervalos propuestos'!$E$3:$E$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>1.8464555865077115E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5488285801558477E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1339404543395446E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5405554786504858E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.861410975446065E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.411553244548692E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9928097326246008E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4499390410438795E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6996802499655517E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2465822272314102E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7855731346684065E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2528171559232359E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2653342394252984E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5992626733667414E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.958287330209485E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9443783600047393E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.740227397717109E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0512659653128429E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.3392021204187206E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.006084982533296E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.8071113181189591E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.9362577136936565E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5933966830937729E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.1819024573725199E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.7609709574213444E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.7028324269193993E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.4545521517898785E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.4372543362244148E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.047231807107976E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.4586274342798577E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.8882110810163E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.3183749251233294E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.7782747633616647E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.3647336399046694E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.0786124867182627E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.3542555230794737E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.6988720462365881E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.7368542718371405E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.5697641157323194E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.5933966830937729E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.9738379125890493E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.1714556779486527E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.740227397717109E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.861410975446065E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.8438796155143597E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.4858957604453216E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.0474878538684349E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.3780909163713004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-51BB-465F-9B2F-8D0A0DAF67A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intervalos propuestos'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Superior</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intervalos propuestos'!$F$3:$F$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>6.6502590428620278E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7478812792070991E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0131485534768455E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3168264260430854E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9055701752429751E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9865880475373505E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3390765979019546E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6556371699174315E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11743907636986073</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4324485196669464E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4652583497444871E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.128872845880738</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.10502449496865905</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.3574655205062849E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.0054134380961979E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.7034192539259449E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.6350813646779553E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.6330936165841884E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.6214920629670961E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.8970952423400181E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.6880919492669391E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.7724423014538334E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.0308632478614584E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.5897816608143996E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.6648430365609452E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.4186838650892623E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.1445980706064643E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.8977307187676487E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.0845626424668862E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.4857754252320987E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.3986217274952807E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.5358889203911186E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.9525991761323707E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.2589900693957065E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.2894482434461677E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.6574956178320581E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.6797412621892994E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.0356594105307885E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.11043169002348147</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.1452882234430183E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.6746772909233318E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9.0962990926360121E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.5479388634965616E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.6658075997594211E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.7614089485154246E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.5692966787837093E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.8301445094402512E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.2814717628659723E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-51BB-465F-9B2F-8D0A0DAF67A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intervalos propuestos'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exigente </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intervalos propuestos'!$H$3:$H$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>4.2483573146848697E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1483549296814734E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5735445039081951E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9286909523467856E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3834905753445201E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1990706460430212E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6659431652632773E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0527881054806555E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.7217939434758123E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8395153734491783E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1254157422064471E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0700508719985178E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.3838918681456025E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.9783640969365132E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9818503841528415E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.3238988069653421E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6876543811975318E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.8421797909485156E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.7277061375044841E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.5488518702966739E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.2476016336929495E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.8543500075737449E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.3121299654776157E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.8858420590934598E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.3204700661515402E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.0607581460043308E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2995751111981714E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.6674925274960317E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.2446429115888423E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.9722014297559782E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.6434164042557907E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.7338632064517258E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.8654369697470177E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.811861854650188E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.598654746058997E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5058755704557659E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6893066542129441E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.3862568411839641E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.306466559040233E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.3693424532683956E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.8242576017561906E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.6338773852923324E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.6440831306068353E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.7636092876027427E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.2728984550334303E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.0275962196145154E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.4388161816543431E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.8297813396186363E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-51BB-465F-9B2F-8D0A0DAF67A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:axId val="441986992"/>
+        <c:axId val="441993232"/>
+      </c:stockChart>
+      <c:catAx>
+        <c:axId val="441986992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441993232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="441993232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441986992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -16404,6 +18048,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17141,7 +18786,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -17181,6 +18826,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18159,6 +19805,86 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -20779,6 +22505,1038 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="323">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -21298,7 +24056,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="323">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -21987,6 +24745,159 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>752474</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.05236</cdr:x>
+      <cdr:y>0.69594</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.98429</cdr:x>
+      <cdr:y>0.70118</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="Conector recto 2"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="381000" y="2528888"/>
+          <a:ext cx="6781800" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04849</cdr:x>
+      <cdr:y>0.63444</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.98952</cdr:x>
+      <cdr:y>0.63709</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="Conector recto 2"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="352426" y="2281238"/>
+          <a:ext cx="6838950" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>51</xdr:row>
@@ -27076,7 +29987,7 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30442,16 +33353,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C50:K50">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K49">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>"0.05"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:J49">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30461,7 +33377,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="8" id="{F0E5EDA9-07DA-4AB7-BE05-20B60A455445}">
+          <x14:cfRule type="expression" priority="9" id="{F0E5EDA9-07DA-4AB7-BE05-20B60A455445}">
             <xm:f>C2&gt;'Intervalos propuestos'!#REF!</xm:f>
             <x14:dxf>
               <fill>
@@ -30484,8 +33400,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30504,8 +33420,10 @@
         <v>62</v>
       </c>
       <c r="F1" s="13"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -30526,8 +33444,12 @@
       <c r="F2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -30548,7 +33470,12 @@
       <c r="F3">
         <v>6.6502590428620278E-2</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3">
+        <v>4.784634623520212E-2</v>
+      </c>
+      <c r="H3">
+        <v>4.2483573146848697E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -30569,7 +33496,12 @@
       <c r="F4">
         <v>6.7478812792070991E-2</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <v>4.4849436759287667E-2</v>
+      </c>
+      <c r="H4">
+        <v>4.1483549296814734E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -30590,7 +33522,12 @@
       <c r="F5">
         <v>5.0131485534768455E-2</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <v>3.9536326733484527E-2</v>
+      </c>
+      <c r="H5">
+        <v>3.5735445039081951E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -30611,7 +33548,12 @@
       <c r="F6">
         <v>7.3168264260430854E-2</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>5.6400807482371536E-2</v>
+      </c>
+      <c r="H6">
+        <v>4.9286909523467856E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -30632,7 +33574,12 @@
       <c r="F7">
         <v>4.9055701752429751E-2</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3">
+        <v>3.8783296932426527E-2</v>
+      </c>
+      <c r="H7">
+        <v>3.3834905753445201E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -30653,7 +33600,12 @@
       <c r="F8">
         <v>7.9865880475373505E-2</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3">
+        <v>6.0780117513283494E-2</v>
+      </c>
+      <c r="H8">
+        <v>5.1990706460430212E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -30674,7 +33626,12 @@
       <c r="F9">
         <v>5.3390765979019546E-2</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3">
+        <v>4.075959116743548E-2</v>
+      </c>
+      <c r="H9">
+        <v>3.6659431652632773E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -30695,7 +33652,12 @@
       <c r="F10">
         <v>4.6556371699174315E-2</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3">
+        <v>3.3741098816488839E-2</v>
+      </c>
+      <c r="H10">
+        <v>3.0527881054806555E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -30716,7 +33678,12 @@
       <c r="F11">
         <v>0.11743907636986073</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3">
+        <v>7.5015277646548445E-2</v>
+      </c>
+      <c r="H11">
+        <v>6.7217939434758123E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -30737,7 +33704,12 @@
       <c r="F12">
         <v>5.4324485196669464E-2</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <v>5.2778173279380725E-2</v>
+      </c>
+      <c r="H12">
+        <v>4.8395153734491783E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -30758,7 +33730,12 @@
       <c r="F13">
         <v>3.4652583497444871E-2</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3">
+        <v>3.4522053559650649E-2</v>
+      </c>
+      <c r="H13">
+        <v>3.1254157422064471E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -30779,7 +33756,12 @@
       <c r="F14">
         <v>0.128872845880738</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3">
+        <v>7.9960081080267364E-2</v>
+      </c>
+      <c r="H14">
+        <v>7.0700508719985178E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -30800,7 +33782,12 @@
       <c r="F15">
         <v>0.10502449496865905</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3">
+        <v>6.7430003561988833E-2</v>
+      </c>
+      <c r="H15">
+        <v>6.3838918681456025E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -30821,9 +33808,14 @@
       <c r="F16">
         <v>6.3574655205062849E-2</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3">
+        <v>4.3924695802630455E-2</v>
+      </c>
+      <c r="H16">
+        <v>3.9783640969365132E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -30842,9 +33834,14 @@
       <c r="F17">
         <v>6.0054134380961979E-2</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3">
+        <v>4.1016515002253964E-2</v>
+      </c>
+      <c r="H17">
+        <v>3.9818503841528415E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -30863,9 +33860,14 @@
       <c r="F18">
         <v>6.7034192539259449E-2</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3">
+        <v>4.6599866235643557E-2</v>
+      </c>
+      <c r="H18">
+        <v>4.3238988069653421E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -30884,9 +33886,14 @@
       <c r="F19">
         <v>5.6350813646779553E-2</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3">
+        <v>4.1783317483531188E-2</v>
+      </c>
+      <c r="H19">
+        <v>3.6876543811975318E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -30905,9 +33912,14 @@
       <c r="F20">
         <v>7.6330936165841884E-2</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3">
+        <v>5.6241283025071823E-2</v>
+      </c>
+      <c r="H20">
+        <v>4.8421797909485156E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -30926,9 +33938,14 @@
       <c r="F21">
         <v>4.6214920629670961E-2</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3">
+        <v>2.9516069015001548E-2</v>
+      </c>
+      <c r="H21">
+        <v>2.7277061375044841E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -30947,9 +33964,14 @@
       <c r="F22">
         <v>4.8970952423400181E-2</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="3">
+        <v>3.5278968361034252E-2</v>
+      </c>
+      <c r="H22">
+        <v>2.5488518702966739E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -30968,9 +33990,14 @@
       <c r="F23">
         <v>4.6880919492669391E-2</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="G23" s="3">
+        <v>3.6531447400988126E-2</v>
+      </c>
+      <c r="H23">
+        <v>3.2476016336929495E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -30989,9 +34016,14 @@
       <c r="F24">
         <v>9.7724423014538334E-2</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3">
+        <v>6.62265629928835E-2</v>
+      </c>
+      <c r="H24">
+        <v>5.8543500075737449E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -31010,9 +34042,14 @@
       <c r="F25">
         <v>5.0308632478614584E-2</v>
       </c>
-      <c r="G25" s="3"/>
+      <c r="G25" s="3">
+        <v>4.233048970564024E-2</v>
+      </c>
+      <c r="H25">
+        <v>3.3121299654776157E-2</v>
+      </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -31031,9 +34068,14 @@
       <c r="F26">
         <v>5.5897816608143996E-2</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="3">
+        <v>4.0825647020573272E-2</v>
+      </c>
+      <c r="H26">
+        <v>3.8858420590934598E-2</v>
+      </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -31052,9 +34094,14 @@
       <c r="F27">
         <v>5.6648430365609452E-2</v>
       </c>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3">
+        <v>3.9575393695157599E-2</v>
+      </c>
+      <c r="H27">
+        <v>3.3204700661515402E-2</v>
+      </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -31073,9 +34120,14 @@
       <c r="F28">
         <v>7.4186838650892623E-2</v>
       </c>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3">
+        <v>5.744877001040033E-2</v>
+      </c>
+      <c r="H28">
+        <v>5.0607581460043308E-2</v>
+      </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -31094,9 +34146,14 @@
       <c r="F29">
         <v>7.1445980706064643E-2</v>
       </c>
-      <c r="G29" s="3"/>
+      <c r="G29" s="3">
+        <v>4.9277977676795301E-2</v>
+      </c>
+      <c r="H29">
+        <v>4.2995751111981714E-2</v>
+      </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -31115,9 +34172,14 @@
       <c r="F30">
         <v>6.8977307187676487E-2</v>
       </c>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3">
+        <v>5.1556006014235031E-2</v>
+      </c>
+      <c r="H30">
+        <v>4.6674925274960317E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -31136,9 +34198,14 @@
       <c r="F31">
         <v>6.0845626424668862E-2</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="3">
+        <v>3.7431736160829766E-2</v>
+      </c>
+      <c r="H31">
+        <v>3.2446429115888423E-2</v>
+      </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -31157,9 +34224,14 @@
       <c r="F32">
         <v>6.4857754252320987E-2</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3">
+        <v>4.5588796895214355E-2</v>
+      </c>
+      <c r="H32">
+        <v>3.9722014297559782E-2</v>
+      </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -31178,9 +34250,14 @@
       <c r="F33">
         <v>5.3986217274952807E-2</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3">
+        <v>4.1652261064670071E-2</v>
+      </c>
+      <c r="H33">
+        <v>3.6434164042557907E-2</v>
+      </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -31199,9 +34276,14 @@
       <c r="F34">
         <v>4.5358889203911186E-2</v>
       </c>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3">
+        <v>3.3828196417877793E-2</v>
+      </c>
+      <c r="H34">
+        <v>2.7338632064517258E-2</v>
+      </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -31220,9 +34302,14 @@
       <c r="F35">
         <v>9.9525991761323707E-2</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="G35" s="3">
+        <v>6.4619957788938129E-2</v>
+      </c>
+      <c r="H35">
+        <v>5.8654369697470177E-2</v>
+      </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -31241,9 +34328,14 @@
       <c r="F36">
         <v>4.2589900693957065E-2</v>
       </c>
-      <c r="G36" s="3"/>
+      <c r="G36" s="3">
+        <v>3.2302964857036626E-2</v>
+      </c>
+      <c r="H36">
+        <v>2.811861854650188E-2</v>
+      </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -31262,9 +34354,14 @@
       <c r="F37">
         <v>6.2894482434461677E-2</v>
       </c>
-      <c r="G37" s="3"/>
+      <c r="G37" s="3">
+        <v>4.3046117063583557E-2</v>
+      </c>
+      <c r="H37">
+        <v>3.598654746058997E-2</v>
+      </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -31283,9 +34380,14 @@
       <c r="F38">
         <v>4.6574956178320581E-2</v>
       </c>
-      <c r="G38" s="3"/>
+      <c r="G38" s="3">
+        <v>4.3129216049080966E-2</v>
+      </c>
+      <c r="H38">
+        <v>3.5058755704557659E-2</v>
+      </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -31304,9 +34406,14 @@
       <c r="F39">
         <v>5.6797412621892994E-2</v>
       </c>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3">
+        <v>4.048694534603417E-2</v>
+      </c>
+      <c r="H39">
+        <v>3.6893066542129441E-2</v>
+      </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -31325,9 +34432,14 @@
       <c r="F40">
         <v>5.0356594105307885E-2</v>
       </c>
-      <c r="G40" s="3"/>
+      <c r="G40" s="3">
+        <v>3.6818986566839754E-2</v>
+      </c>
+      <c r="H40">
+        <v>3.3862568411839641E-2</v>
+      </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -31346,9 +34458,14 @@
       <c r="F41">
         <v>0.11043169002348147</v>
       </c>
-      <c r="G41" s="3"/>
+      <c r="G41" s="3">
+        <v>6.9242789423307777E-2</v>
+      </c>
+      <c r="H41">
+        <v>6.306466559040233E-2</v>
+      </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -31367,9 +34484,14 @@
       <c r="F42">
         <v>9.1452882234430183E-2</v>
       </c>
-      <c r="G42" s="3"/>
+      <c r="G42" s="3">
+        <v>6.103440843630864E-2</v>
+      </c>
+      <c r="H42">
+        <v>5.3693424532683956E-2</v>
+      </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -31388,9 +34510,14 @@
       <c r="F43">
         <v>7.6746772909233318E-2</v>
       </c>
-      <c r="G43" s="3"/>
+      <c r="G43" s="3">
+        <v>5.0601755241498812E-2</v>
+      </c>
+      <c r="H43">
+        <v>4.8242576017561906E-2</v>
+      </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -31409,9 +34536,14 @@
       <c r="F44">
         <v>9.0962990926360121E-2</v>
       </c>
-      <c r="G44" s="3"/>
+      <c r="G44" s="3">
+        <v>5.8718604532877187E-2</v>
+      </c>
+      <c r="H44">
+        <v>5.6338773852923324E-2</v>
+      </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -31430,9 +34562,14 @@
       <c r="F45">
         <v>7.5479388634965616E-2</v>
       </c>
-      <c r="G45" s="3"/>
+      <c r="G45" s="3">
+        <v>5.9152421314825607E-2</v>
+      </c>
+      <c r="H45">
+        <v>4.6440831306068353E-2</v>
+      </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -31451,9 +34588,14 @@
       <c r="F46">
         <v>5.6658075997594211E-2</v>
       </c>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3">
+        <v>4.2399605609261683E-2</v>
+      </c>
+      <c r="H46">
+        <v>3.7636092876027427E-2</v>
+      </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -31472,9 +34614,14 @@
       <c r="F47">
         <v>3.7614089485154246E-2</v>
       </c>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3">
+        <v>2.9391724191112932E-2</v>
+      </c>
+      <c r="H47">
+        <v>2.2728984550334303E-2</v>
+      </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -31493,9 +34640,14 @@
       <c r="F48">
         <v>6.5692966787837093E-2</v>
       </c>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3">
+        <v>4.3886407771377742E-2</v>
+      </c>
+      <c r="H48">
+        <v>4.0275962196145154E-2</v>
+      </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -31514,9 +34666,14 @@
       <c r="F49">
         <v>4.8301445094402512E-2</v>
       </c>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3">
+        <v>3.8890622076086456E-2</v>
+      </c>
+      <c r="H49">
+        <v>3.4388161816543431E-2</v>
+      </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -31535,15 +34692,22 @@
       <c r="F50">
         <v>7.2814717628659723E-2</v>
       </c>
-      <c r="G50" s="3"/>
+      <c r="G50" s="3">
+        <v>5.7266018588752958E-2</v>
+      </c>
+      <c r="H50">
+        <v>4.8297813396186363E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -31552,7 +34716,7 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
@@ -31570,42 +34734,42 @@
       <c r="B1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16" t="s">
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16" t="s">
+      <c r="N1" s="14"/>
+      <c r="O1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="15" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="15"/>
-      <c r="S1" s="14" t="s">
+      <c r="R1" s="16"/>
+      <c r="S1" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="T1" s="14"/>
+      <c r="T1" s="15"/>
       <c r="U1" s="13" t="s">
         <v>60</v>
       </c>
@@ -36227,16 +39391,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>